<commit_message>
apply confspace and create dany q agent
</commit_message>
<xml_diff>
--- a/Python/code/RL/env/grid/map/Dyna Q Test.xlsx
+++ b/Python/code/RL/env/grid/map/Dyna Q Test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MH\frozen-lake2\Python\code\rl\env\grid\map\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E2609B-C007-4CA9-9CCD-FCA8807361CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{952A64FC-17B0-43B0-83F2-D08036CBB652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5385" windowWidth="29040" windowHeight="15840" xr2:uid="{59FFA0EA-9011-4021-B407-57F9149DDA9D}"/>
+    <workbookView xWindow="-28920" yWindow="5385" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{59FFA0EA-9011-4021-B407-57F9149DDA9D}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="5" r:id="rId1"/>
@@ -518,7 +518,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{233CEAA4-6FD9-4CF1-9EE9-AFD117D3CDAA}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
@@ -602,8 +602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBE4013A-13DA-4A32-839D-2876A9DEEA13}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -649,12 +649,13 @@
       <c r="F4" t="s">
         <v>2</v>
       </c>
+      <c r="G4" t="s">
+        <v>2</v>
+      </c>
       <c r="H4" t="s">
         <v>2</v>
       </c>
-      <c r="I4" s="5" t="s">
-        <v>2</v>
-      </c>
+      <c r="I4" s="5"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A5" s="4"/>

</xml_diff>